<commit_message>
ajustes dos scripts knn
</commit_message>
<xml_diff>
--- a/KNN - Nearest Neighbors/01 - Algoritimo Paciente com Gripe/dados_gripe.xlsx
+++ b/KNN - Nearest Neighbors/01 - Algoritimo Paciente com Gripe/dados_gripe.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22185" windowHeight="9210"/>
+    <workbookView windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha2" sheetId="2" r:id="rId1"/>
@@ -210,8 +210,16 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -683,141 +691,144 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1366,7 +1377,7 @@
   <sheetPr/>
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1385,31 +1396,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4258,5 +4269,8 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <ignoredErrors>
+    <ignoredError sqref="A2:I99" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>